<commit_message>
Correction in: feil i commongarden
</commit_message>
<xml_diff>
--- a/Data/Feil i commongarden.xlsx
+++ b/Data/Feil i commongarden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livvel\Documents\Callunachildren\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D76F92-361B-4797-B9F6-67888AE958EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3894C593-E261-4ABF-A128-5DEA0C0920DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{7A255D68-551B-456F-80E7-13EE14ADD2E7}"/>
   </bookViews>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840EAEFD-B9E0-40B2-9B60-4063677C96A0}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1701,7 +1701,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="6">
-        <v>4772</v>
+        <v>1238</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>8</v>

</xml_diff>